<commit_message>
added initial instructions and parts list
</commit_message>
<xml_diff>
--- a/docs/partslist.xlsx
+++ b/docs/partslist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\picodistance\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8E9B43-CD6C-40F4-928B-F0A847C9193E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8412249E-BCA2-497B-A602-29D712B3A10B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="170" windowWidth="19380" windowHeight="11200" xr2:uid="{CD05D57E-1B61-436F-89D7-0F69D0E55BF9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{CD05D57E-1B61-436F-89D7-0F69D0E55BF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>Item</t>
   </si>
@@ -50,18 +50,12 @@
     <t>3621AS</t>
   </si>
   <si>
-    <t>LED 2-Digit 7-Segment Display</t>
-  </si>
-  <si>
     <t>Datasheet</t>
   </si>
   <si>
     <t>http://www.xlitx.com/datasheet/3621AS.pdf</t>
   </si>
   <si>
-    <t>LED 4-Digit 7-Segment Display</t>
-  </si>
-  <si>
     <t>3641AH</t>
   </si>
   <si>
@@ -107,9 +101,6 @@
     <t>https://drive.google.com/file/d/1rvWWXi3pNAfMBGfCexUg1QRdRRH0I-_h/view?pli=1</t>
   </si>
   <si>
-    <t>Mini Level Picture Hanging Spirit Bubble Level, 10x10x29mm Square Level Mark Measuring Tools</t>
-  </si>
-  <si>
     <t>‎43338-2313</t>
   </si>
   <si>
@@ -141,6 +132,27 @@
   </si>
   <si>
     <t>Surface Mounted Devices Chip Resistor, 220 Ohm 1/10W Fixed Resistors</t>
+  </si>
+  <si>
+    <t>Mini Level Picture Hanging Spirit Bubble Level, 10x10x29mm Square Level Mark Measuring Tool</t>
+  </si>
+  <si>
+    <t>3MM flat top white LED</t>
+  </si>
+  <si>
+    <t>AA00136</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.us/item/2251832094868310.html?pdp_npi=2%40dis%21USD%21US%20%245.70%21US%20%243.99%21%21%21%21%21%40211b88f016829744756592864ef47c%2112000015876525887%21sh&amp;gatewayAdapt=glo2usa</t>
+  </si>
+  <si>
+    <t>LED 2-Digit 7-Segment Display 0.36"</t>
+  </si>
+  <si>
+    <t>LED 4-Digit 7-Segment Display 0.36"</t>
+  </si>
+  <si>
+    <t>5vDC voltage regulator</t>
   </si>
 </sst>
 </file>
@@ -511,17 +523,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29BCD5B8-3994-48AF-A8BF-C030B66F4D4C}">
-  <dimension ref="A2:D14"/>
+  <dimension ref="A2:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="31.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" style="2"/>
+    <col min="2" max="2" width="15.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39.90625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -529,164 +541,193 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="1">
+        <v>7805</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="C5" s="2">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:4" ht="87" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="2">
-        <v>2</v>
+        <v>33</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1">
+        <v>4</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="2">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1">
         <v>2</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="2">
-        <v>1</v>
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="2">
-        <v>3</v>
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="2">
+        <v>19</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="1">
         <v>2</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>25</v>
+      <c r="D10" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="2">
-        <v>1</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="2">
+      <c r="C13" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>32</v>
+      <c r="D13" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -694,11 +735,12 @@
     <hyperlink ref="D3" r:id="rId1" xr:uid="{2D37A1B2-5717-40E5-82E1-17363A656F53}"/>
     <hyperlink ref="D4" r:id="rId2" xr:uid="{1D2FC12D-C9BA-40DC-A579-C728AD7A65B5}"/>
     <hyperlink ref="D5" r:id="rId3" xr:uid="{4665727D-92C2-453D-879A-216DA6400ED4}"/>
-    <hyperlink ref="D6" r:id="rId4" xr:uid="{CCCC683A-DE8C-41EE-A0D9-9205C183B29D}"/>
-    <hyperlink ref="D8" r:id="rId5" location="dzXcwUN_xoUTOmhmVMA0sg/folder/E5BFULaB" xr:uid="{02EE287C-8D3B-4ACE-A64E-2F1395DBDC64}"/>
-    <hyperlink ref="D7" r:id="rId6" location="74hc595n-pinout-diagram" xr:uid="{B7FFB24A-EA5A-46B9-B414-2E22CD0146C8}"/>
-    <hyperlink ref="D9" r:id="rId7" xr:uid="{4F6D14E8-7230-422C-A717-D4238FD2DD4F}"/>
-    <hyperlink ref="D11" r:id="rId8" xr:uid="{2C5977F3-4AB1-42F3-94C1-41C4B7EA3C35}"/>
+    <hyperlink ref="D7" r:id="rId4" xr:uid="{CCCC683A-DE8C-41EE-A0D9-9205C183B29D}"/>
+    <hyperlink ref="D9" r:id="rId5" location="dzXcwUN_xoUTOmhmVMA0sg/folder/E5BFULaB" xr:uid="{02EE287C-8D3B-4ACE-A64E-2F1395DBDC64}"/>
+    <hyperlink ref="D8" r:id="rId6" location="74hc595n-pinout-diagram" xr:uid="{B7FFB24A-EA5A-46B9-B414-2E22CD0146C8}"/>
+    <hyperlink ref="D10" r:id="rId7" xr:uid="{4F6D14E8-7230-422C-A717-D4238FD2DD4F}"/>
+    <hyperlink ref="D12" r:id="rId8" xr:uid="{2C5977F3-4AB1-42F3-94C1-41C4B7EA3C35}"/>
+    <hyperlink ref="D6" r:id="rId9" xr:uid="{FD77E920-23FA-4FFB-B532-A1C67DD23491}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>